<commit_message>
# Conclusions 16 - adding different learning rates. Default in tf.keras.optimizers.Adam is 0.001, tried with 0.0001 - Took longer - 400-600 seconds (vs 200-300 with 0.001) - Many more epochs - 55-80 - Accuracy was not great - product .98-.99 (stop function stops before reached the best result?) ### Conclusions going forward: - Try with larger rate to see if will give same results as 0.001 but quicker.  Try 0.02 as suggested in the lecture
</commit_message>
<xml_diff>
--- a/output/16_learn_rate_0.0001/best.xlsx
+++ b/output/16_learn_rate_0.0001/best.xlsx
@@ -484,7 +484,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F2" t="n">
         <v>200</v>
@@ -507,34 +507,34 @@
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9902999997138977</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9884999990463257</v>
+        <v>0.9814000129699707</v>
       </c>
       <c r="N2" t="n">
-        <v>465.913</v>
+        <v>432.465</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0021</v>
+        <v>0.0023</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0021</v>
+        <v>0.0023</v>
       </c>
       <c r="Q2" t="n">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R2" t="n">
-        <v>6.9539</v>
+        <v>8.008599999999999</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9901999831199646</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.991100013256073</v>
       </c>
       <c r="U2" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.991100013256073</v>
       </c>
     </row>
     <row r="3">
@@ -553,7 +553,7 @@
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F3" t="n">
         <v>200</v>
@@ -573,37 +573,37 @@
         <v>0.0001</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9980000257492065</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9884999990463257</v>
+        <v>0.9959999918937683</v>
       </c>
       <c r="N3" t="n">
-        <v>465.913</v>
+        <v>631.567</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0021</v>
+        <v>0.0016</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0021</v>
+        <v>0.0016</v>
       </c>
       <c r="Q3" t="n">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="R3" t="n">
-        <v>6.9539</v>
+        <v>7.8946</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9977999925613403</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.9980000257492065</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.9980000257492065</v>
       </c>
     </row>
     <row r="4">
@@ -622,7 +622,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F4" t="n">
         <v>200</v>
@@ -645,34 +645,34 @@
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9902999997138977</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9884999990463257</v>
+        <v>0.9814000129699707</v>
       </c>
       <c r="N4" t="n">
-        <v>465.913</v>
+        <v>432.465</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0021</v>
+        <v>0.0023</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0021</v>
+        <v>0.0023</v>
       </c>
       <c r="Q4" t="n">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R4" t="n">
-        <v>6.9539</v>
+        <v>8.008599999999999</v>
       </c>
       <c r="S4" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9901999831199646</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.991100013256073</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.991100013256073</v>
       </c>
     </row>
     <row r="5">
@@ -691,7 +691,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F5" t="n">
         <v>200</v>
@@ -711,37 +711,37 @@
         <v>0.0001</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L5" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9980000257492065</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9884999990463257</v>
+        <v>0.9959999918937683</v>
       </c>
       <c r="N5" t="n">
-        <v>465.913</v>
+        <v>631.567</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0021</v>
+        <v>0.0016</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0021</v>
+        <v>0.0016</v>
       </c>
       <c r="Q5" t="n">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="R5" t="n">
-        <v>6.9539</v>
+        <v>7.8946</v>
       </c>
       <c r="S5" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9977999925613403</v>
       </c>
       <c r="T5" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.9980000257492065</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.9980000257492065</v>
       </c>
     </row>
     <row r="6">
@@ -760,7 +760,7 @@
         <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F6" t="n">
         <v>200</v>
@@ -783,34 +783,34 @@
         <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9902999997138977</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9884999990463257</v>
+        <v>0.9814000129699707</v>
       </c>
       <c r="N6" t="n">
-        <v>465.913</v>
+        <v>432.465</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0021</v>
+        <v>0.0023</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0021</v>
+        <v>0.0023</v>
       </c>
       <c r="Q6" t="n">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R6" t="n">
-        <v>6.9539</v>
+        <v>8.008599999999999</v>
       </c>
       <c r="S6" t="n">
-        <v>0.9941999912261963</v>
+        <v>0.9901999831199646</v>
       </c>
       <c r="T6" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.991100013256073</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9943000078201294</v>
+        <v>0.991100013256073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>